<commit_message>
feat: Started PROG1500 A-01 Database Design and SQL
</commit_message>
<xml_diff>
--- a/Courses/PROG1500 - Databases and SQL/Modules/Module 1 - SQL and Data/Assignments/Assignment1_3NFTable.xlsx
+++ b/Courses/PROG1500 - Databases and SQL/Modules/Module 1 - SQL and Data/Assignments/Assignment1_3NFTable.xlsx
@@ -1,34 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vreed\Desktop\Ryan\OTech\Software_Technology\Courses\PROG1500 - Databases and SQL\Modules\Module 1 - SQL and Data\Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4400113921\Desktop\Ryan\Software_Technology\Courses\PROG1500 - Databases and SQL\Modules\Module 1 - SQL and Data\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEA848C-36F8-463A-98A9-5753EF069082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF99D518-66F9-4D8F-B67B-7FFEA93B5A23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="student" sheetId="1" r:id="rId1"/>
+    <sheet name="student_class" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
-  <si>
-    <t>StudentID</t>
-  </si>
-  <si>
-    <t>StudentName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="34">
   <si>
     <t>Certificate</t>
   </si>
@@ -36,30 +30,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>ClassRoomNumber</t>
-  </si>
-  <si>
-    <t>ClassTime</t>
-  </si>
-  <si>
-    <t>ClassID</t>
-  </si>
-  <si>
-    <t>ClassTitle</t>
-  </si>
-  <si>
-    <t>StudentStartDate</t>
-  </si>
-  <si>
-    <t>ProgressScheduled</t>
-  </si>
-  <si>
-    <t>ProgressCompleted</t>
-  </si>
-  <si>
-    <t>ProgressPrecent</t>
-  </si>
-  <si>
     <t>Kevin S. Barker</t>
   </si>
   <si>
@@ -121,13 +91,46 @@
   </si>
   <si>
     <t>Ogden Weber Students</t>
+  </si>
+  <si>
+    <t>Student_ID</t>
+  </si>
+  <si>
+    <t>Student_Name</t>
+  </si>
+  <si>
+    <t>Class_Room_Number</t>
+  </si>
+  <si>
+    <t>Class_Time</t>
+  </si>
+  <si>
+    <t>Class_ID</t>
+  </si>
+  <si>
+    <t>Class_Title</t>
+  </si>
+  <si>
+    <t>Student_Start_Date</t>
+  </si>
+  <si>
+    <t>Progress_Scheduled</t>
+  </si>
+  <si>
+    <t>Progress_Completed</t>
+  </si>
+  <si>
+    <t>Progress_Precent</t>
+  </si>
+  <si>
+    <t>PK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,8 +146,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +171,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -181,11 +203,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,8 +222,27 @@
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
@@ -538,69 +580,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M15"/>
+  <dimension ref="B1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -608,16 +650,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2">
         <v>0.33333333333333331</v>
@@ -626,7 +668,7 @@
         <v>158.80000000000001</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="J4" s="3">
         <v>41598</v>
@@ -643,209 +685,209 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G5" s="2">
-        <v>0.33333333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="H5" s="1">
-        <v>158.80000000000001</v>
+        <v>158.9</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="J5" s="3">
-        <v>41978</v>
+        <v>41598</v>
       </c>
       <c r="K5" s="1">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="L5" s="1">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M5" s="4">
-        <v>0.8</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="G6" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H6" s="1">
-        <v>148.1</v>
+        <v>158.80000000000001</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="J6" s="3">
-        <v>41561</v>
+        <v>41978</v>
       </c>
       <c r="K6" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="L6" s="1">
         <v>12</v>
       </c>
       <c r="M6" s="4">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="H7" s="1">
-        <v>148.1</v>
+        <v>158.9</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="J7" s="3">
-        <v>41528</v>
+        <v>41978</v>
       </c>
       <c r="K7" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L7" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M7" s="4">
-        <v>1.25</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H8" s="1">
+        <v>148.1</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="H8" s="1">
-        <v>158.80000000000001</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="J8" s="3">
-        <v>41580</v>
+        <v>41561</v>
       </c>
       <c r="K8" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L8" s="1">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="M8" s="4">
-        <v>2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H9" s="1">
+        <v>148.11000000000001</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="H9" s="1">
-        <v>158.80000000000001</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="J9" s="3">
-        <v>41570</v>
+        <v>41561</v>
       </c>
       <c r="K9" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L9" s="1">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M9" s="4">
-        <v>0.95</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G10" s="2">
         <v>0.41666666666666669</v>
@@ -854,213 +896,922 @@
         <v>148.1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J10" s="3">
-        <v>41596</v>
+        <v>41528</v>
       </c>
       <c r="K10" s="1">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="L10" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="M10" s="4">
-        <v>2.14</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H11" s="1">
+        <v>148.11000000000001</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="J11" s="3">
+        <v>41528</v>
+      </c>
+      <c r="K11" s="1">
+        <v>12</v>
+      </c>
+      <c r="L11" s="1">
         <v>15</v>
       </c>
-      <c r="G11" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="H11" s="1">
-        <v>158.9</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="3">
-        <v>41570</v>
-      </c>
-      <c r="K11" s="1">
-        <v>20</v>
-      </c>
-      <c r="L11" s="1">
-        <v>19</v>
-      </c>
       <c r="M11" s="4">
-        <v>0.95</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H12" s="1">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="3">
+        <v>41580</v>
+      </c>
+      <c r="K12" s="1">
+        <v>40</v>
+      </c>
+      <c r="L12" s="1">
+        <v>80</v>
+      </c>
+      <c r="M12" s="4">
         <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="H12" s="1">
-        <v>158.9</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="3">
-        <v>41978</v>
-      </c>
-      <c r="K12" s="1">
-        <v>15</v>
-      </c>
-      <c r="L12" s="1">
-        <v>12</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0.8</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H13" s="1">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="3">
+        <v>41570</v>
+      </c>
+      <c r="K13" s="1">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="H13" s="1">
-        <v>148.11000000000001</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="3">
-        <v>41561</v>
-      </c>
-      <c r="K13" s="1">
-        <v>30</v>
-      </c>
       <c r="L13" s="1">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M13" s="4">
-        <v>0.4</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="H14" s="1">
+        <v>158.9</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="3">
+        <v>41570</v>
+      </c>
+      <c r="K14" s="1">
         <v>20</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="H14" s="1">
-        <v>148.11000000000001</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="3">
-        <v>41528</v>
-      </c>
-      <c r="K14" s="1">
-        <v>12</v>
-      </c>
       <c r="L14" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="M14" s="4">
-        <v>1.25</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H15" s="1">
+        <v>148.1</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="3">
+        <v>41596</v>
+      </c>
+      <c r="K15" s="1">
+        <v>28</v>
+      </c>
+      <c r="L15" s="1">
+        <v>60</v>
+      </c>
+      <c r="M15" s="4">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="str">
+        <f>LOWER(B3)</f>
+        <v>student_id</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" ref="C18:M18" si="0">LOWER(C3)</f>
+        <v>student_name</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>certificate</v>
+      </c>
+      <c r="E18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>phone</v>
+      </c>
+      <c r="F18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>class_room_number</v>
+      </c>
+      <c r="G18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>class_time</v>
+      </c>
+      <c r="H18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>class_id</v>
+      </c>
+      <c r="I18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>class_title</v>
+      </c>
+      <c r="J18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>student_start_date</v>
+      </c>
+      <c r="K18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>progress_scheduled</v>
+      </c>
+      <c r="L18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>progress_completed</v>
+      </c>
+      <c r="M18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>progress_precent</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H19" s="6">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="8">
+        <v>41598</v>
+      </c>
+      <c r="K19" s="5">
+        <v>23</v>
+      </c>
+      <c r="L19" s="5">
+        <v>20</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="H20" s="6">
+        <v>158.9</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="8">
+        <v>41598</v>
+      </c>
+      <c r="K20" s="5">
+        <v>23</v>
+      </c>
+      <c r="L20" s="5">
+        <v>20</v>
+      </c>
+      <c r="M20" s="9">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>2</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H21" s="6">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="8">
+        <v>41978</v>
+      </c>
+      <c r="K21" s="5">
+        <v>15</v>
+      </c>
+      <c r="L21" s="5">
+        <v>12</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="H22" s="6">
+        <v>158.9</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="8">
+        <v>41978</v>
+      </c>
+      <c r="K22" s="5">
+        <v>15</v>
+      </c>
+      <c r="L22" s="5">
+        <v>12</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>3</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H23" s="6">
+        <v>148.1</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="J23" s="8">
+        <v>41561</v>
+      </c>
+      <c r="K23" s="5">
+        <v>30</v>
+      </c>
+      <c r="L23" s="5">
+        <v>12</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>3</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H24" s="6">
+        <v>148.11000000000001</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="8">
+        <v>41561</v>
+      </c>
+      <c r="K24" s="5">
+        <v>30</v>
+      </c>
+      <c r="L24" s="5">
+        <v>12</v>
+      </c>
+      <c r="M24" s="9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="D25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="2">
+      <c r="F25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H25" s="6">
+        <v>148.1</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="8">
+        <v>41528</v>
+      </c>
+      <c r="K25" s="5">
+        <v>12</v>
+      </c>
+      <c r="L25" s="5">
+        <v>15</v>
+      </c>
+      <c r="M25" s="9">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H26" s="6">
+        <v>148.11000000000001</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="8">
+        <v>41528</v>
+      </c>
+      <c r="K26" s="5">
+        <v>12</v>
+      </c>
+      <c r="L26" s="5">
+        <v>15</v>
+      </c>
+      <c r="M26" s="9">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H27" s="6">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="8">
+        <v>41580</v>
+      </c>
+      <c r="K27" s="5">
+        <v>40</v>
+      </c>
+      <c r="L27" s="5">
+        <v>80</v>
+      </c>
+      <c r="M27" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H28" s="6">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" s="8">
+        <v>41570</v>
+      </c>
+      <c r="K28" s="5">
+        <v>20</v>
+      </c>
+      <c r="L28" s="5">
+        <v>19</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>6</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="7">
         <v>0.375</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H29" s="6">
         <v>158.9</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="8">
+        <v>41570</v>
+      </c>
+      <c r="K29" s="5">
+        <v>20</v>
+      </c>
+      <c r="L29" s="5">
+        <v>19</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <v>7</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H30" s="6">
+        <v>148.1</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="8">
+        <v>41596</v>
+      </c>
+      <c r="K30" s="5">
+        <v>28</v>
+      </c>
+      <c r="L30" s="5">
+        <v>60</v>
+      </c>
+      <c r="M30" s="9">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="str">
+        <f>LOWER(B18)</f>
+        <v>student_id</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <f t="shared" ref="C33:F33" si="1">LOWER(C18)</f>
+        <v>student_name</v>
+      </c>
+      <c r="D33" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>certificate</v>
+      </c>
+      <c r="E33" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>phone</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
+        <v>2</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <v>2</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
+        <v>3</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
+        <v>3</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="6">
+        <v>4</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="6">
+        <v>4</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="6">
+        <v>5</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="3">
-        <v>41598</v>
-      </c>
-      <c r="K15" s="1">
-        <v>23</v>
-      </c>
-      <c r="L15" s="1">
+      <c r="D42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="6">
+        <v>6</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="6">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="6">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M15" s="4">
-        <v>0.87</v>
+      <c r="D45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B4:M15">
+    <sortCondition ref="B4"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>